<commit_message>
untidy data with species codes and answer key example
</commit_message>
<xml_diff>
--- a/Week01_Spreadsheets/untidy-portal-data.xlsx
+++ b/Week01_Spreadsheets/untidy-portal-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebledsoe/Documents/Git/DataWrangling/Week01_Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40CBB0EB-2237-F94D-8045-61207E6F4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED254C-AFB9-BE44-B41E-05279CCD17FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28120" windowHeight="18760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
   <si>
     <t>Data for Site 7</t>
   </si>
@@ -174,6 +174,24 @@
   </si>
   <si>
     <t>Dipodomys on Plot 4</t>
+  </si>
+  <si>
+    <t>Species Code</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>DX</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>DO</t>
   </si>
 </sst>
 </file>
@@ -606,15 +624,15 @@
   <dimension ref="A3:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.5" customWidth="1"/>
     <col min="14" max="14" width="17.83203125" customWidth="1"/>
   </cols>
@@ -628,7 +646,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>2</v>
       </c>
       <c r="M5" t="s">
@@ -640,28 +658,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="I6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
       <c r="J6" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
@@ -681,28 +696,25 @@
         <v>41648</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1">
-        <v>41647</v>
+      <c r="F7" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="K7">
         <v>-999</v>
@@ -722,28 +734,25 @@
         <v>41648</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1">
-        <v>41647</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
       <c r="I8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="K8">
         <v>44</v>
@@ -763,28 +772,25 @@
         <v>41648</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1">
-        <v>41647</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="K9">
         <v>38</v>
@@ -804,28 +810,25 @@
         <v>41648</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="1">
-        <v>41647</v>
+      <c r="F10" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="K10">
         <v>-999</v>
@@ -845,28 +848,25 @@
         <v>41659</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="1">
-        <v>41647</v>
+      <c r="F11" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>220</v>
@@ -886,28 +886,25 @@
         <v>41659</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="1">
-        <v>41647</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
       <c r="I12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K12">
         <v>38</v>
@@ -927,22 +924,19 @@
         <v>41711</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="1">
-        <v>41647</v>
-      </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K13">
         <v>48</v>
@@ -962,22 +956,19 @@
         <v>41711</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="1">
-        <v>41647</v>
+      <c r="F14" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K14">
         <v>143</v>
@@ -994,22 +985,19 @@
         <v>41711</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="1">
-        <v>41647</v>
+      <c r="F15" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K15">
         <v>35</v>
@@ -1019,11 +1007,14 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G16" s="1">
-        <v>41647</v>
+      <c r="F16" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K16">
         <v>43</v>
@@ -1039,11 +1030,14 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G17" s="1">
-        <v>41647</v>
+      <c r="F17" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K17">
         <v>37</v>
@@ -1059,11 +1053,14 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G18" s="1">
-        <v>41647</v>
+      <c r="F18" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K18">
         <v>150</v>
@@ -1079,11 +1076,14 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G19" s="1">
-        <v>41647</v>
+      <c r="F19" s="1">
+        <v>41647</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K19">
         <v>45</v>
@@ -1099,34 +1099,40 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G20" s="1">
-        <v>41647</v>
+      <c r="F20" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="K20">
         <v>-999</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="G21" s="1">
-        <v>41647</v>
+      <c r="F21" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J21" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K21" s="3">
         <v>157</v>
@@ -1136,17 +1142,20 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="1">
-        <v>41647</v>
+      <c r="F22" s="1">
+        <v>41647</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="J22" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="K22">
         <v>-999</v>
@@ -1165,17 +1174,20 @@
       <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="1">
+      <c r="F23" s="1">
         <v>41688</v>
       </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="K23" s="3">
         <v>218</v>
@@ -1186,7 +1198,7 @@
         <v>38</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1194,17 +1206,20 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="G24" s="1">
+      <c r="F24" s="1">
         <v>41688</v>
       </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
       <c r="H24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K24" s="3">
         <v>127</v>
@@ -1223,17 +1238,20 @@
       <c r="D25">
         <v>7</v>
       </c>
-      <c r="G25" s="1">
+      <c r="F25" s="1">
         <v>41688</v>
       </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
       <c r="H25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K25" s="3">
         <v>52</v>
@@ -1258,7 +1276,7 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1272,14 +1290,14 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
-      <c r="G29" s="3"/>
-      <c r="H29" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
include untidy excel file
</commit_message>
<xml_diff>
--- a/Week01_Spreadsheets/untidy-portal-data.xlsx
+++ b/Week01_Spreadsheets/untidy-portal-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebledsoe/Documents/Git/DataWrangling/Week01_Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED254C-AFB9-BE44-B41E-05279CCD17FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B92D8A3-695D-964D-B237-CA7C535286EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28120" windowHeight="18760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A3:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>